<commit_message>
Add header to phm.xlsx and minor bug fixes.
</commit_message>
<xml_diff>
--- a/phm.xlsx
+++ b/phm.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,22 +24,22 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.3499862666707358"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -47,12 +47,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,204 +520,287 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col width="12.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="2.73046875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="21.86328125" bestFit="1" customWidth="1" min="4" max="5"/>
-    <col width="11.1328125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="12.33203125" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="7.1328125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="10" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="21.86328125" bestFit="1" customWidth="1" style="1" min="4" max="5"/>
+    <col width="11.1328125" bestFit="1" customWidth="1" style="1" min="6" max="6"/>
+    <col width="10.53125" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="9.06640625" customWidth="1" style="1" min="8" max="24"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="14.65" customFormat="1" customHeight="1" s="1" thickBot="1">
+      <c r="A1" s="11" t="inlineStr">
+        <is>
+          <t>Table Name</t>
+        </is>
+      </c>
+      <c r="B1" s="11" t="inlineStr">
+        <is>
+          <t>Number</t>
+        </is>
+      </c>
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="11" t="inlineStr">
+        <is>
+          <t>Start Time</t>
+        </is>
+      </c>
+      <c r="E1" s="11" t="inlineStr">
+        <is>
+          <t>Update Time</t>
+        </is>
+      </c>
+      <c r="F1" s="11" t="inlineStr">
+        <is>
+          <t>Elapsed Time</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="inlineStr">
+        <is>
+          <t>Current Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="1">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_1</t>
         </is>
       </c>
-      <c r="B1" t="n">
+      <c r="B2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D2" s="9" t="n"/>
+      <c r="E2" s="7" t="n"/>
+      <c r="F2" s="7" t="n"/>
+      <c r="G2" s="3" t="n"/>
+    </row>
+    <row r="3" customFormat="1" s="1">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_2</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr"/>
+      <c r="E3" s="7" t="inlineStr"/>
+      <c r="F3" s="7" t="inlineStr"/>
+      <c r="G3" s="3" t="inlineStr"/>
+    </row>
+    <row r="4" customFormat="1" s="1">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_3</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="n"/>
+      <c r="E4" s="7" t="n"/>
+      <c r="F4" s="7" t="n"/>
+      <c r="G4" s="3" t="n"/>
+    </row>
+    <row r="5" customFormat="1" s="1">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_4</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D5" s="9" t="inlineStr"/>
+      <c r="E5" s="7" t="inlineStr"/>
+      <c r="F5" s="7" t="inlineStr"/>
+      <c r="G5" s="3" t="inlineStr"/>
+    </row>
+    <row r="6" customFormat="1" s="1">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_5</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B6" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="n"/>
+      <c r="E6" s="7" t="n"/>
+      <c r="F6" s="7" t="n"/>
+      <c r="G6" s="3" t="n"/>
+    </row>
+    <row r="7" customFormat="1" s="1">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_6</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="n"/>
+      <c r="E7" s="7" t="n"/>
+      <c r="F7" s="7" t="n"/>
+      <c r="G7" s="3" t="n"/>
+    </row>
+    <row r="8" customFormat="1" s="1">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_7</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B8" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D8" s="9" t="n"/>
+      <c r="E8" s="7" t="n"/>
+      <c r="F8" s="7" t="n"/>
+      <c r="G8" s="3" t="n"/>
+    </row>
+    <row r="9" customFormat="1" s="1">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_8</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B9" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D9" s="9" t="n"/>
+      <c r="E9" s="7" t="n"/>
+      <c r="F9" s="7" t="n"/>
+      <c r="G9" s="3" t="n"/>
+    </row>
+    <row r="10" customFormat="1" s="1">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_9</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D10" s="9" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="3" t="inlineStr"/>
+    </row>
+    <row r="11" customFormat="1" s="1">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_10</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B11" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D11" s="9" t="n"/>
+      <c r="E11" s="7" t="n"/>
+      <c r="F11" s="7" t="n"/>
+      <c r="G11" s="3" t="n"/>
+    </row>
+    <row r="12" customFormat="1" s="1">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>Pool_Table_11</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B12" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D12" s="9" t="n"/>
+      <c r="E12" s="7" t="n"/>
+      <c r="F12" s="7" t="n"/>
+      <c r="G12" s="3" t="n"/>
+    </row>
+    <row r="13" ht="14.65" customFormat="1" customHeight="1" s="1" thickBot="1">
+      <c r="A13" s="8" t="inlineStr">
         <is>
           <t>Pool_Table_12</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Unoccupied</t>
-        </is>
-      </c>
+      <c r="C13" s="8" t="inlineStr">
+        <is>
+          <t>Unoccupied</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="n"/>
+      <c r="E13" s="8" t="n"/>
+      <c r="F13" s="8" t="n"/>
+      <c r="G13" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>